<commit_message>
improve error handling with file system
</commit_message>
<xml_diff>
--- a/RR calculation.xlsx
+++ b/RR calculation.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z004fxaa\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jinji\Desktop\BinanceBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F418167B-2C9B-4A68-9E7E-32E513700559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{38A0CE40-613D-4B29-B956-06D8C2D9F672}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -66,10 +65,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -121,15 +120,15 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -137,6 +136,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -452,26 +452,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92B3330-C39B-4AC0-808E-1E325A068D91}">
-  <dimension ref="C1:H14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="46.36328125" customWidth="1"/>
-    <col min="5" max="5" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="3:9" x14ac:dyDescent="0.25">
       <c r="H1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>1</v>
       </c>
@@ -486,7 +486,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>0</v>
       </c>
@@ -498,28 +498,36 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="9">
-        <v>2.9999999999999997E-4</v>
+        <v>1.5E-3</v>
       </c>
       <c r="E6" s="3">
         <f>E2/D6</f>
-        <v>3333.3333333333335</v>
+        <v>666.66666666666663</v>
       </c>
       <c r="G6" s="10">
         <f>E6*D6</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="H6" s="11">
+        <f>D6*H2</f>
+        <v>2.2500000000000003E-3</v>
+      </c>
+      <c r="I6" s="10">
+        <f>E6*H6</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E7" s="5">
         <f>E6*D6</f>
         <v>1</v>
@@ -528,12 +536,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C10" s="4" t="s">
         <v>4</v>
       </c>
@@ -544,8 +552,20 @@
         <f>E2/D10</f>
         <v>12.5</v>
       </c>
-    </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="G10" s="10">
+        <f>E10*D10</f>
+        <v>1</v>
+      </c>
+      <c r="H10" s="11">
+        <f>D10*H2</f>
+        <v>0.12</v>
+      </c>
+      <c r="I10" s="10">
+        <f>E10*H10</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E11" s="5">
         <f>E10*D10</f>
         <v>1</v>
@@ -554,7 +574,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="3:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:9" ht="75" x14ac:dyDescent="0.25">
       <c r="D14" s="7" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
added lowest stop loss percentage
</commit_message>
<xml_diff>
--- a/RR calculation.xlsx
+++ b/RR calculation.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Rolling capital</t>
   </si>
@@ -60,17 +60,32 @@
     <t>1st step Firm R=10 = Y ; 
 2nd step &gt; keep update every trade's Risk % = X,
 Final = placement bet amount = Y/X</t>
+  </si>
+  <si>
+    <t>commission</t>
+  </si>
+  <si>
+    <t>Win</t>
+  </si>
+  <si>
+    <t>Lose</t>
+  </si>
+  <si>
+    <t>Net</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0.0000%"/>
+    <numFmt numFmtId="167" formatCode="0.00000%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,8 +100,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -105,13 +128,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -120,7 +160,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -134,9 +174,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -453,25 +503,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:I14"/>
+  <dimension ref="C1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="46.42578125" customWidth="1"/>
     <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:16" x14ac:dyDescent="0.25">
       <c r="H1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>1</v>
       </c>
@@ -486,48 +538,80 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>0</v>
       </c>
-      <c r="E3">
-        <v>1000</v>
-      </c>
-      <c r="F3" s="8">
+      <c r="F3" s="8" t="e">
         <f>E2/E3</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="M4" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" s="15"/>
+      <c r="P4" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="M5" s="13">
+        <f>H2</f>
+        <v>1.5</v>
+      </c>
+      <c r="N5" s="13">
+        <f>E2</f>
+        <v>1</v>
+      </c>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="9">
-        <v>1.5E-3</v>
+      <c r="D6" s="14">
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="E6" s="3">
         <f>E2/D6</f>
-        <v>666.66666666666663</v>
-      </c>
-      <c r="G6" s="10">
+        <v>400</v>
+      </c>
+      <c r="G6" s="9">
         <f>E6*D6</f>
         <v>1</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="10">
         <f>D6*H2</f>
-        <v>2.2500000000000003E-3</v>
-      </c>
-      <c r="I6" s="10">
+        <v>3.7499999999999999E-3</v>
+      </c>
+      <c r="I6" s="9">
         <f>E6*H6</f>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6" s="13">
+        <f>E6*(0.00027*2)</f>
+        <v>0.216</v>
+      </c>
+      <c r="N6" s="13">
+        <f>M6</f>
+        <v>0.216</v>
+      </c>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+    </row>
+    <row r="7" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E7" s="5">
         <f>E6*D6</f>
         <v>1</v>
@@ -535,13 +619,33 @@
       <c r="F7" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="M7" s="17">
+        <f>M5-M6</f>
+        <v>1.284</v>
+      </c>
+      <c r="N7" s="17">
+        <f>SUM(N5:N6)</f>
+        <v>1.216</v>
+      </c>
+      <c r="O7" s="13"/>
+      <c r="P7" s="17">
+        <f>M7-N7</f>
+        <v>6.800000000000006E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="P8" s="9">
+        <f>P7/E2</f>
+        <v>6.800000000000006E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="M9" s="9"/>
+    </row>
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C10" s="4" t="s">
         <v>4</v>
       </c>
@@ -552,20 +656,20 @@
         <f>E2/D10</f>
         <v>12.5</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="9">
         <f>E10*D10</f>
         <v>1</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="10">
         <f>D10*H2</f>
         <v>0.12</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="9">
         <f>E10*H10</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E11" s="5">
         <f>E10*D10</f>
         <v>1</v>
@@ -574,15 +678,31 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="3:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:16" ht="75" x14ac:dyDescent="0.25">
       <c r="D14" s="7" t="s">
         <v>7</v>
       </c>
     </row>
+    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="E16" s="9">
+        <f>460*0.0004</f>
+        <v>0.184</v>
+      </c>
+      <c r="F16" s="9">
+        <f>E16*2</f>
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G17" s="11"/>
+      <c r="H17" s="12"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <customProperties>
-    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId1"/>
+    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId2"/>
   </customProperties>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "added lowest stop loss percentage"
This reverts commit ba2ffdd0378806abd576be78ece5516915e374be.
</commit_message>
<xml_diff>
--- a/RR calculation.xlsx
+++ b/RR calculation.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>Rolling capital</t>
   </si>
@@ -60,32 +60,17 @@
     <t>1st step Firm R=10 = Y ; 
 2nd step &gt; keep update every trade's Risk % = X,
 Final = placement bet amount = Y/X</t>
-  </si>
-  <si>
-    <t>commission</t>
-  </si>
-  <si>
-    <t>Win</t>
-  </si>
-  <si>
-    <t>Lose</t>
-  </si>
-  <si>
-    <t>Net</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
-    <numFmt numFmtId="166" formatCode="0.0000%"/>
-    <numFmt numFmtId="167" formatCode="0.00000%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,16 +85,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -128,30 +105,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -160,7 +120,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -174,19 +134,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -503,27 +453,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:P17"/>
+  <dimension ref="C1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="46.42578125" customWidth="1"/>
     <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:9" x14ac:dyDescent="0.25">
       <c r="H1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>1</v>
       </c>
@@ -538,80 +486,48 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="8" t="e">
+      <c r="E3">
+        <v>1000</v>
+      </c>
+      <c r="F3" s="8">
         <f>E2/E3</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="M4" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="N4" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="O4" s="15"/>
-      <c r="P4" s="16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="13">
-        <f>H2</f>
-        <v>1.5</v>
-      </c>
-      <c r="N5" s="13">
-        <f>E2</f>
-        <v>1</v>
-      </c>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-    </row>
-    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="14">
-        <v>2.5000000000000001E-3</v>
+      <c r="D6" s="9">
+        <v>1.5E-3</v>
       </c>
       <c r="E6" s="3">
         <f>E2/D6</f>
-        <v>400</v>
-      </c>
-      <c r="G6" s="9">
+        <v>666.66666666666663</v>
+      </c>
+      <c r="G6" s="10">
         <f>E6*D6</f>
         <v>1</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="11">
         <f>D6*H2</f>
-        <v>3.7499999999999999E-3</v>
-      </c>
-      <c r="I6" s="9">
+        <v>2.2500000000000003E-3</v>
+      </c>
+      <c r="I6" s="10">
         <f>E6*H6</f>
         <v>1.5</v>
       </c>
-      <c r="L6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M6" s="13">
-        <f>E6*(0.00027*2)</f>
-        <v>0.216</v>
-      </c>
-      <c r="N6" s="13">
-        <f>M6</f>
-        <v>0.216</v>
-      </c>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-    </row>
-    <row r="7" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E7" s="5">
         <f>E6*D6</f>
         <v>1</v>
@@ -619,33 +535,13 @@
       <c r="F7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="17">
-        <f>M5-M6</f>
-        <v>1.284</v>
-      </c>
-      <c r="N7" s="17">
-        <f>SUM(N5:N6)</f>
-        <v>1.216</v>
-      </c>
-      <c r="O7" s="13"/>
-      <c r="P7" s="17">
-        <f>M7-N7</f>
-        <v>6.800000000000006E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="P8" s="9">
-        <f>P7/E2</f>
-        <v>6.800000000000006E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>5</v>
       </c>
-      <c r="M9" s="9"/>
-    </row>
-    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C10" s="4" t="s">
         <v>4</v>
       </c>
@@ -656,20 +552,20 @@
         <f>E2/D10</f>
         <v>12.5</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="10">
         <f>E10*D10</f>
         <v>1</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="11">
         <f>D10*H2</f>
         <v>0.12</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="10">
         <f>E10*H10</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E11" s="5">
         <f>E10*D10</f>
         <v>1</v>
@@ -678,31 +574,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="3:16" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:9" ht="75" x14ac:dyDescent="0.25">
       <c r="D14" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="E16" s="9">
-        <f>460*0.0004</f>
-        <v>0.184</v>
-      </c>
-      <c r="F16" s="9">
-        <f>E16*2</f>
-        <v>0.36799999999999999</v>
-      </c>
-      <c r="G16" s="13"/>
-    </row>
-    <row r="17" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G17" s="11"/>
-      <c r="H17" s="12"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <customProperties>
-    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId2"/>
+    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId1"/>
   </customProperties>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Revert "added lowest stop loss percentage""
This reverts commit 74b238b0c71f8eb9c77a19a2f795a69b377b4270.
</commit_message>
<xml_diff>
--- a/RR calculation.xlsx
+++ b/RR calculation.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Rolling capital</t>
   </si>
@@ -60,17 +60,32 @@
     <t>1st step Firm R=10 = Y ; 
 2nd step &gt; keep update every trade's Risk % = X,
 Final = placement bet amount = Y/X</t>
+  </si>
+  <si>
+    <t>commission</t>
+  </si>
+  <si>
+    <t>Win</t>
+  </si>
+  <si>
+    <t>Lose</t>
+  </si>
+  <si>
+    <t>Net</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0.0000%"/>
+    <numFmt numFmtId="167" formatCode="0.00000%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,8 +100,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -105,13 +128,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -120,7 +160,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -134,9 +174,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -453,25 +503,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:I14"/>
+  <dimension ref="C1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="46.42578125" customWidth="1"/>
     <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:16" x14ac:dyDescent="0.25">
       <c r="H1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>1</v>
       </c>
@@ -486,48 +538,80 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>0</v>
       </c>
-      <c r="E3">
-        <v>1000</v>
-      </c>
-      <c r="F3" s="8">
+      <c r="F3" s="8" t="e">
         <f>E2/E3</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="M4" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" s="15"/>
+      <c r="P4" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="M5" s="13">
+        <f>H2</f>
+        <v>1.5</v>
+      </c>
+      <c r="N5" s="13">
+        <f>E2</f>
+        <v>1</v>
+      </c>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="9">
-        <v>1.5E-3</v>
+      <c r="D6" s="14">
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="E6" s="3">
         <f>E2/D6</f>
-        <v>666.66666666666663</v>
-      </c>
-      <c r="G6" s="10">
+        <v>400</v>
+      </c>
+      <c r="G6" s="9">
         <f>E6*D6</f>
         <v>1</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="10">
         <f>D6*H2</f>
-        <v>2.2500000000000003E-3</v>
-      </c>
-      <c r="I6" s="10">
+        <v>3.7499999999999999E-3</v>
+      </c>
+      <c r="I6" s="9">
         <f>E6*H6</f>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6" s="13">
+        <f>E6*(0.00027*2)</f>
+        <v>0.216</v>
+      </c>
+      <c r="N6" s="13">
+        <f>M6</f>
+        <v>0.216</v>
+      </c>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+    </row>
+    <row r="7" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E7" s="5">
         <f>E6*D6</f>
         <v>1</v>
@@ -535,13 +619,33 @@
       <c r="F7" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="M7" s="17">
+        <f>M5-M6</f>
+        <v>1.284</v>
+      </c>
+      <c r="N7" s="17">
+        <f>SUM(N5:N6)</f>
+        <v>1.216</v>
+      </c>
+      <c r="O7" s="13"/>
+      <c r="P7" s="17">
+        <f>M7-N7</f>
+        <v>6.800000000000006E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="P8" s="9">
+        <f>P7/E2</f>
+        <v>6.800000000000006E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="M9" s="9"/>
+    </row>
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C10" s="4" t="s">
         <v>4</v>
       </c>
@@ -552,20 +656,20 @@
         <f>E2/D10</f>
         <v>12.5</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="9">
         <f>E10*D10</f>
         <v>1</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="10">
         <f>D10*H2</f>
         <v>0.12</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="9">
         <f>E10*H10</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E11" s="5">
         <f>E10*D10</f>
         <v>1</v>
@@ -574,15 +678,31 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="3:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:16" ht="75" x14ac:dyDescent="0.25">
       <c r="D14" s="7" t="s">
         <v>7</v>
       </c>
     </row>
+    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="E16" s="9">
+        <f>460*0.0004</f>
+        <v>0.184</v>
+      </c>
+      <c r="F16" s="9">
+        <f>E16*2</f>
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G17" s="11"/>
+      <c r="H17" s="12"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <customProperties>
-    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId1"/>
+    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId2"/>
   </customProperties>
 </worksheet>
 </file>
</xml_diff>